<commit_message>
Calculations on sample data
</commit_message>
<xml_diff>
--- a/Giant Eagle Data Stuff.xlsx
+++ b/Giant Eagle Data Stuff.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="EVERYTHING" sheetId="1" r:id="rId1"/>
@@ -189,18 +189,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -227,24 +221,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -274,6 +267,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -286,9 +282,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,11 +822,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1281819056"/>
-        <c:axId val="1281818512"/>
+        <c:axId val="5891680"/>
+        <c:axId val="176947504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1281819056"/>
+        <c:axId val="5891680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1281818512"/>
+        <c:crossAx val="176947504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -938,7 +933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1281818512"/>
+        <c:axId val="176947504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1281819056"/>
+        <c:crossAx val="5891680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1325,11 +1320,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1489718272"/>
-        <c:axId val="1489732960"/>
+        <c:axId val="236706768"/>
+        <c:axId val="236705680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1489718272"/>
+        <c:axId val="236706768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1371,7 +1366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1489732960"/>
+        <c:crossAx val="236705680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1379,7 +1374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1489732960"/>
+        <c:axId val="236705680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1425,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1489718272"/>
+        <c:crossAx val="236706768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1519,7 +1514,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1850,11 +1844,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1110341952"/>
-        <c:axId val="1110344672"/>
+        <c:axId val="235535312"/>
+        <c:axId val="235534224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1110341952"/>
+        <c:axId val="235535312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,7 +1890,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1110344672"/>
+        <c:crossAx val="235534224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1904,7 +1898,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1110344672"/>
+        <c:axId val="235534224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1955,7 +1949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1110341952"/>
+        <c:crossAx val="235535312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2044,7 +2038,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2171,11 +2164,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1335525824"/>
-        <c:axId val="1335539424"/>
+        <c:axId val="235532048"/>
+        <c:axId val="235544016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1335525824"/>
+        <c:axId val="235532048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2217,7 +2210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1335539424"/>
+        <c:crossAx val="235544016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2225,7 +2218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1335539424"/>
+        <c:axId val="235544016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2276,7 +2269,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1335525824"/>
+        <c:crossAx val="235532048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2365,7 +2358,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2555,11 +2547,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1335533440"/>
-        <c:axId val="1335531808"/>
+        <c:axId val="235539120"/>
+        <c:axId val="235545104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1335533440"/>
+        <c:axId val="235539120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2601,7 +2593,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1335531808"/>
+        <c:crossAx val="235545104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2609,7 +2601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1335531808"/>
+        <c:axId val="235545104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2660,7 +2652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1335533440"/>
+        <c:crossAx val="235539120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2749,7 +2741,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2939,11 +2930,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1335532352"/>
-        <c:axId val="1335524736"/>
+        <c:axId val="235531504"/>
+        <c:axId val="235539664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1335532352"/>
+        <c:axId val="235531504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2985,7 +2976,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1335524736"/>
+        <c:crossAx val="235539664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2993,7 +2984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1335524736"/>
+        <c:axId val="235539664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,7 +3035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1335532352"/>
+        <c:crossAx val="235531504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3614,11 +3605,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1050482880"/>
-        <c:axId val="1050487232"/>
+        <c:axId val="235540752"/>
+        <c:axId val="235536400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1050482880"/>
+        <c:axId val="235540752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3716,7 +3707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050487232"/>
+        <c:crossAx val="235536400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3725,7 +3716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1050487232"/>
+        <c:axId val="235536400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3832,7 +3823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050482880"/>
+        <c:crossAx val="235540752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4253,11 +4244,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1281809264"/>
-        <c:axId val="1281809808"/>
+        <c:axId val="235541296"/>
+        <c:axId val="235533680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1281809264"/>
+        <c:axId val="235541296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4299,7 +4290,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1281809808"/>
+        <c:crossAx val="235533680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4307,7 +4298,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1281809808"/>
+        <c:axId val="235533680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4358,7 +4349,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1281809264"/>
+        <c:crossAx val="235541296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4447,7 +4438,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4574,11 +4564,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1050486688"/>
-        <c:axId val="1050485600"/>
+        <c:axId val="235538576"/>
+        <c:axId val="235538032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1050486688"/>
+        <c:axId val="235538576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4620,7 +4610,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050485600"/>
+        <c:crossAx val="235538032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4628,7 +4618,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1050485600"/>
+        <c:axId val="235538032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4679,7 +4669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1050486688"/>
+        <c:crossAx val="235538576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4768,7 +4758,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4958,11 +4947,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1489719904"/>
-        <c:axId val="1489728064"/>
+        <c:axId val="236692080"/>
+        <c:axId val="236696432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1489719904"/>
+        <c:axId val="236692080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5004,7 +4993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1489728064"/>
+        <c:crossAx val="236696432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5012,7 +5001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1489728064"/>
+        <c:axId val="236696432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5063,7 +5052,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1489719904"/>
+        <c:crossAx val="236692080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11135,10 +11124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J239"/>
+  <dimension ref="A1:J249"/>
   <sheetViews>
-    <sheetView topLeftCell="B82" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E45"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E249" sqref="A249:E249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -11156,7 +11145,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -11172,10 +11161,10 @@
         <v>8</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -11185,7 +11174,7 @@
       </c>
       <c r="B2">
         <f>AVERAGE(A2:A239)</f>
-        <v>20.344537815126049</v>
+        <v>22.483193277310924</v>
       </c>
       <c r="D2" s="2">
         <v>6</v>
@@ -11197,11 +11186,11 @@
         <f>E2/D2</f>
         <v>11.333333333333334</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <f>AVERAGE(E2:E45)</f>
         <v>115.5</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <f>AVERAGE(G2:G45)</f>
         <v>28.765203045617486</v>
       </c>
@@ -11223,7 +11212,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -11366,7 +11355,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -11382,7 +11371,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2">
         <v>5</v>
@@ -11398,7 +11387,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2">
         <v>14</v>
@@ -11414,7 +11403,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2">
         <v>4</v>
@@ -11510,7 +11499,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -11526,7 +11515,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
@@ -11542,7 +11531,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -11558,7 +11547,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" s="2">
         <v>4</v>
@@ -11574,7 +11563,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
@@ -11590,7 +11579,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="2">
         <v>5</v>
@@ -11624,7 +11613,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2">
         <v>5</v>
@@ -11640,7 +11629,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2">
         <v>2</v>
@@ -11656,7 +11645,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
@@ -11672,7 +11661,7 @@
     </row>
     <row r="32" spans="1:7" ht="12.75">
       <c r="A32" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2">
         <v>5</v>
@@ -11688,7 +11677,7 @@
     </row>
     <row r="33" spans="1:7" ht="12.75">
       <c r="A33" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D33" s="2">
         <v>6</v>
@@ -11706,7 +11695,7 @@
     </row>
     <row r="34" spans="1:7" ht="12.75">
       <c r="A34" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34" s="2">
         <v>9</v>
@@ -11722,7 +11711,7 @@
     </row>
     <row r="35" spans="1:7" ht="12.75">
       <c r="A35" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2">
         <v>3</v>
@@ -11738,7 +11727,7 @@
     </row>
     <row r="36" spans="1:7" ht="12.75">
       <c r="A36" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36" s="2">
         <v>12</v>
@@ -11836,7 +11825,7 @@
     </row>
     <row r="42" spans="1:7" ht="12.75">
       <c r="A42" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
@@ -11852,7 +11841,7 @@
     </row>
     <row r="43" spans="1:7" ht="12.75">
       <c r="A43" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D43" s="2">
         <v>11</v>
@@ -11868,7 +11857,7 @@
     </row>
     <row r="44" spans="1:7" ht="12.75">
       <c r="A44" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D44" s="2">
         <v>8</v>
@@ -11886,7 +11875,7 @@
     </row>
     <row r="45" spans="1:7" ht="12.75">
       <c r="A45" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D45" s="2">
         <v>2</v>
@@ -11902,754 +11891,768 @@
     </row>
     <row r="46" spans="1:7" ht="12.75">
       <c r="A46" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="12.75">
       <c r="A47" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="12.75">
       <c r="A48" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="12.75">
       <c r="A49" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="12.75">
       <c r="A50" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="12.75">
       <c r="A51" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="12.75">
       <c r="A52" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="12.75">
       <c r="A53" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="12.75">
       <c r="A54" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="12.75">
       <c r="A55" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="12.75">
       <c r="A56" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="12.75">
       <c r="A57" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="12.75">
       <c r="A58" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="12.75">
       <c r="A59" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="12.75">
       <c r="A60" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="12.75">
       <c r="A61" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="12.75">
       <c r="A62" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="12.75">
       <c r="A63" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="12.75">
       <c r="A64" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="12.75">
       <c r="A65" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="12.75">
       <c r="A66" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="12.75">
       <c r="A67" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="12.75">
       <c r="A68" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="12.75">
       <c r="A69" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="12.75">
       <c r="A70" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="12.75">
       <c r="A71" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="12.75">
       <c r="A72" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="12.75">
       <c r="A73" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="12.75">
       <c r="A74" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="12.75">
       <c r="A75" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="12.75">
       <c r="A76" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="12.75">
       <c r="A77" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="12.75">
       <c r="A78" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="12.75">
       <c r="A79" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="12.75">
       <c r="A80" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="12.75">
       <c r="A81" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="12.75">
       <c r="A82" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="12.75">
       <c r="A83" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="12.75">
       <c r="A84" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="12.75">
       <c r="A85" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="12.75">
       <c r="A86" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="12.75">
       <c r="A87" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="12.75">
       <c r="A88" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="12.75">
       <c r="A89" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="12.75">
       <c r="A90" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="12.75">
       <c r="A91" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" ht="12.75">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="12.75">
       <c r="A92" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="12.75">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="12.75">
       <c r="A93" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" ht="12.75">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="12.75">
       <c r="A94" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" ht="12.75">
+        <v>11</v>
+      </c>
+      <c r="D94" s="26"/>
+    </row>
+    <row r="95" spans="1:4" ht="12.75">
       <c r="A95" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" ht="12.75">
+        <v>12</v>
+      </c>
+      <c r="D95" s="26"/>
+    </row>
+    <row r="96" spans="1:4" ht="12.75">
       <c r="A96" s="2">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D96" s="26"/>
     </row>
     <row r="97" spans="1:4" ht="12.75">
       <c r="A97" s="2">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D97" s="26"/>
     </row>
     <row r="98" spans="1:4" ht="12.75">
       <c r="A98" s="2">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D98" s="26"/>
     </row>
     <row r="99" spans="1:4" ht="12.75">
       <c r="A99" s="2">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D99" s="26"/>
     </row>
     <row r="100" spans="1:4" ht="12.75">
       <c r="A100" s="2">
-        <v>10</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D100" s="26"/>
     </row>
     <row r="101" spans="1:4" ht="12.75">
       <c r="A101" s="2">
-        <v>10</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D101" s="26"/>
     </row>
     <row r="102" spans="1:4" ht="12.75">
       <c r="A102" s="2">
-        <v>10</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D102" s="26"/>
     </row>
     <row r="103" spans="1:4" ht="14.25">
       <c r="A103" s="2">
-        <v>10</v>
-      </c>
-      <c r="D103" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="D103" s="27"/>
     </row>
     <row r="104" spans="1:4" ht="12.75">
       <c r="A104" s="2">
-        <v>10</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D104" s="26"/>
     </row>
     <row r="105" spans="1:4" ht="14.25">
       <c r="A105" s="2">
-        <v>10</v>
-      </c>
-      <c r="D105" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="D105" s="27"/>
     </row>
     <row r="106" spans="1:4" ht="12.75">
       <c r="A106" s="2">
-        <v>10</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D106" s="26"/>
     </row>
     <row r="107" spans="1:4" ht="12.75">
       <c r="A107" s="2">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D107" s="26"/>
     </row>
     <row r="108" spans="1:4" ht="12.75">
       <c r="A108" s="2">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D108" s="26"/>
     </row>
     <row r="109" spans="1:4" ht="12.75">
       <c r="A109" s="2">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D109" s="26"/>
     </row>
     <row r="110" spans="1:4" ht="12.75">
       <c r="A110" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="12.75">
       <c r="A111" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="12.75">
       <c r="A112" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="12.75">
       <c r="A113" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="12.75">
       <c r="A114" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="12.75">
       <c r="A115" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="12.75">
       <c r="A116" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="12.75">
       <c r="A117" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="12.75">
       <c r="A118" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="12.75">
       <c r="A119" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="12.75">
       <c r="A120" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="12.75">
       <c r="A121" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="12.75">
       <c r="A122" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="12.75">
       <c r="A123" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="12.75">
       <c r="A124" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="12.75">
       <c r="A125" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="12.75">
       <c r="A126" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="12.75">
       <c r="A127" s="2">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="12.75">
       <c r="A128" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="12.75">
       <c r="A129" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="12.75">
       <c r="A130" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="12.75">
       <c r="A131" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="12.75">
       <c r="A132" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="12.75">
       <c r="A133" s="2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="12.75">
       <c r="A134" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="12.75">
       <c r="A135" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="12.75">
       <c r="A136" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="12.75">
       <c r="A137" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="12.75">
       <c r="A138" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="12.75">
       <c r="A139" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="12.75">
       <c r="A140" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="12.75">
       <c r="A141" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="12.75">
-      <c r="A142" s="2">
-        <v>15</v>
+      <c r="A142" s="5">
+        <v>21</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="12.75">
-      <c r="A143" s="2">
-        <v>16</v>
+      <c r="A143" s="5">
+        <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="12.75">
       <c r="A144" s="2">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="12.75">
       <c r="A145" s="2">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="12.75">
       <c r="A146" s="2">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="12.75">
-      <c r="A147" s="2">
-        <v>17</v>
+      <c r="A147" s="5">
+        <v>22</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="12.75">
-      <c r="A148" s="2">
-        <v>17</v>
+      <c r="A148" s="5">
+        <v>22</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="12.75">
       <c r="A149" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="12.75">
       <c r="A150" s="2">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="12.75">
-      <c r="A151" s="2">
-        <v>17</v>
+      <c r="A151" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="12.75">
       <c r="A152" s="2">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="12.75">
-      <c r="A153" s="2">
-        <v>18</v>
+      <c r="A153" s="5">
+        <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="12.75">
-      <c r="A154" s="2">
-        <v>18</v>
+      <c r="A154" s="5">
+        <v>24</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="12.75">
       <c r="A155" s="2">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="12.75">
-      <c r="A156" s="2">
-        <v>18</v>
+      <c r="A156" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="12.75">
       <c r="A157" s="2">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="12.75">
       <c r="A158" s="2">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="12.75">
-      <c r="A159" s="2">
-        <v>19</v>
+      <c r="A159" s="5">
+        <v>26</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="12.75">
       <c r="A160" s="2">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="12.75">
-      <c r="A161" s="2">
-        <v>20</v>
+      <c r="A161" s="5">
+        <v>27</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="12.75">
-      <c r="A162" s="2">
-        <v>20</v>
+      <c r="A162" s="5">
+        <v>27</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="12.75">
-      <c r="A163" s="2">
-        <v>20</v>
+      <c r="A163" s="5">
+        <v>27</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="12.75">
       <c r="A164" s="2">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="12.75">
       <c r="A165" s="2">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="12.75">
       <c r="A166" s="2">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="12.75">
       <c r="A167" s="2">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="12.75">
-      <c r="A168" s="2">
-        <v>21</v>
+      <c r="A168" s="5">
+        <v>28</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="12.75">
-      <c r="A169" s="2">
-        <v>21</v>
+      <c r="A169" s="5">
+        <v>28</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="12.75">
       <c r="A170" s="2">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="12.75">
       <c r="A171" s="2">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="12.75">
-      <c r="A172" s="2">
-        <v>23</v>
+      <c r="A172" s="5">
+        <v>29</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="12.75">
       <c r="A173" s="2">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="12.75">
-      <c r="A174" s="2">
-        <v>25</v>
+      <c r="A174" s="5">
+        <v>30</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="12.75">
-      <c r="A175" s="2">
-        <v>25</v>
+      <c r="A175" s="5">
+        <v>30</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="12.75">
       <c r="A176" s="2">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="12.75">
       <c r="A177" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="12.75">
       <c r="A178" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="12.75">
-      <c r="A179" s="2">
-        <v>27</v>
+      <c r="A179" s="5">
+        <v>31</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="12.75">
       <c r="A180" s="2">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="12.75">
       <c r="A181" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="12.75">
       <c r="A182" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="12.75">
-      <c r="A183" s="2">
-        <v>29</v>
+      <c r="A183" s="5">
+        <v>32</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="12.75">
       <c r="A184" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="185" spans="1:1" ht="12.75">
       <c r="A185" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="186" spans="1:1" ht="12.75">
-      <c r="A186" s="2">
-        <v>30</v>
+      <c r="A186" s="5">
+        <v>33</v>
       </c>
     </row>
     <row r="187" spans="1:1" ht="12.75">
       <c r="A187" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="12.75">
       <c r="A188" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="189" spans="1:1" ht="12.75">
-      <c r="A189" s="2">
-        <v>31</v>
+      <c r="A189" s="5">
+        <v>34</v>
       </c>
     </row>
     <row r="190" spans="1:1" ht="12.75">
-      <c r="A190" s="2">
-        <v>32</v>
+      <c r="A190" s="5">
+        <v>35</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="12.75">
       <c r="A191" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="12.75">
       <c r="A192" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="193" spans="1:1" ht="12.75">
-      <c r="A193" s="2">
-        <v>33</v>
+      <c r="A193" s="5">
+        <v>36</v>
       </c>
     </row>
     <row r="194" spans="1:1" ht="12.75">
-      <c r="A194" s="2">
-        <v>35</v>
+      <c r="A194" s="5">
+        <v>37</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="12.75">
       <c r="A195" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="12.75">
@@ -12663,8 +12666,8 @@
       </c>
     </row>
     <row r="198" spans="1:1" ht="12.75">
-      <c r="A198" s="2">
-        <v>37</v>
+      <c r="A198" s="5">
+        <v>38</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="12.75">
@@ -12678,83 +12681,83 @@
       </c>
     </row>
     <row r="201" spans="1:1" ht="12.75">
-      <c r="A201" s="2">
+      <c r="A201" s="5">
         <v>39</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="12.75">
-      <c r="A202" s="2">
-        <v>40</v>
+      <c r="A202" s="5">
+        <v>39</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="12.75">
       <c r="A203" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="204" spans="1:1" ht="12.75">
-      <c r="A204" s="2">
-        <v>42</v>
+      <c r="A204" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="205" spans="1:1" ht="12.75">
-      <c r="A205" s="2">
-        <v>43</v>
+      <c r="A205" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="206" spans="1:1" ht="12.75">
-      <c r="A206" s="2">
-        <v>44</v>
+      <c r="A206" s="5">
+        <v>40</v>
       </c>
     </row>
     <row r="207" spans="1:1" ht="12.75">
       <c r="A207" s="2">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="208" spans="1:1" ht="12.75">
       <c r="A208" s="2">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="12.75">
       <c r="A209" s="2">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="12.75">
       <c r="A210" s="2">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="211" spans="1:1" ht="12.75">
       <c r="A211" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="212" spans="1:1" ht="12.75">
       <c r="A212" s="2">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="12.75">
       <c r="A213" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="12.75">
       <c r="A214" s="2">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="12.75">
       <c r="A215" s="2">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="12.75">
       <c r="A216" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="12.75">
@@ -12774,7 +12777,7 @@
     </row>
     <row r="220" spans="1:1" ht="12.75">
       <c r="A220" s="2">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="221" spans="1:1" ht="12.75">
@@ -12784,72 +12787,72 @@
     </row>
     <row r="222" spans="1:1" ht="12.75">
       <c r="A222" s="2">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="223" spans="1:1" ht="12.75">
       <c r="A223" s="2">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="224" spans="1:1" ht="12.75">
       <c r="A224" s="2">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="225" spans="1:1" ht="12.75">
-      <c r="A225" s="2">
-        <v>58</v>
+      <c r="A225" s="5">
+        <v>70</v>
       </c>
     </row>
     <row r="226" spans="1:1" ht="12.75">
-      <c r="A226" s="2">
-        <v>58</v>
+      <c r="A226" s="5">
+        <v>70</v>
       </c>
     </row>
     <row r="227" spans="1:1" ht="12.75">
       <c r="A227" s="2">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="228" spans="1:1" ht="12.75">
-      <c r="A228" s="2">
+      <c r="A228" s="5">
         <v>73</v>
       </c>
     </row>
     <row r="229" spans="1:1" ht="12.75">
-      <c r="A229" s="2">
-        <v>76</v>
+      <c r="A229" s="5">
+        <v>75</v>
       </c>
     </row>
     <row r="230" spans="1:1" ht="12.75">
       <c r="A230" s="2">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="231" spans="1:1" ht="12.75">
-      <c r="A231" s="2">
-        <v>79</v>
+      <c r="A231" s="5">
+        <v>77</v>
       </c>
     </row>
     <row r="232" spans="1:1" ht="12.75">
       <c r="A232" s="2">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="233" spans="1:1" ht="12.75">
       <c r="A233" s="2">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="234" spans="1:1" ht="12.75">
-      <c r="A234" s="2">
-        <v>85</v>
+      <c r="A234" s="5">
+        <v>80</v>
       </c>
     </row>
     <row r="235" spans="1:1" ht="12.75">
       <c r="A235" s="2">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="236" spans="1:1" ht="12.75">
@@ -12864,7 +12867,7 @@
     </row>
     <row r="238" spans="1:1" ht="12.75">
       <c r="A238" s="2">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="239" spans="1:1" ht="12.75">
@@ -12872,7 +12875,19 @@
         <v>131</v>
       </c>
     </row>
+    <row r="240" spans="1:1" ht="12.75"/>
+    <row r="241" spans="1:4" ht="12.75"/>
+    <row r="242" spans="1:4" ht="12.75"/>
+    <row r="243" spans="1:4" ht="12.75"/>
+    <row r="244" spans="1:4" ht="12.75"/>
+    <row r="249" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A249" s="5"/>
+      <c r="D249" s="5"/>
+    </row>
   </sheetData>
+  <sortState ref="A2:B239">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12896,16 +12911,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -12919,7 +12934,7 @@
       <c r="D2">
         <v>974.3</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <f>D2/60</f>
         <v>16.238333333333333</v>
       </c>
@@ -12934,7 +12949,7 @@
       <c r="D3">
         <v>470.3</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <f t="shared" ref="E3:E27" si="0">D3/60</f>
         <v>7.8383333333333338</v>
       </c>
@@ -12946,10 +12961,10 @@
       <c r="C4">
         <v>34.200000000000003</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>741.2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f t="shared" si="0"/>
         <v>12.353333333333333</v>
       </c>
@@ -12964,7 +12979,7 @@
       <c r="D5">
         <v>1046.2</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <f t="shared" si="0"/>
         <v>17.436666666666667</v>
       </c>
@@ -12979,7 +12994,7 @@
       <c r="D6">
         <v>1120.4000000000001</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <f t="shared" si="0"/>
         <v>18.673333333333336</v>
       </c>
@@ -12994,7 +13009,7 @@
       <c r="D7">
         <v>952.3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f t="shared" si="0"/>
         <v>15.871666666666666</v>
       </c>
@@ -13009,7 +13024,7 @@
       <c r="D8">
         <v>1309.9000000000001</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <f t="shared" si="0"/>
         <v>21.831666666666667</v>
       </c>
@@ -13024,7 +13039,7 @@
       <c r="D9">
         <v>605</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <f t="shared" si="0"/>
         <v>10.083333333333334</v>
       </c>
@@ -13039,7 +13054,7 @@
       <c r="D10">
         <v>1077.3</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <f t="shared" si="0"/>
         <v>17.954999999999998</v>
       </c>
@@ -13054,7 +13069,7 @@
       <c r="D11">
         <v>1076.2</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <f t="shared" si="0"/>
         <v>17.936666666666667</v>
       </c>
@@ -13069,7 +13084,7 @@
       <c r="D12">
         <v>976.2</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <f t="shared" si="0"/>
         <v>16.27</v>
       </c>
@@ -13084,7 +13099,7 @@
       <c r="D13">
         <v>972.9</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <f t="shared" si="0"/>
         <v>16.215</v>
       </c>
@@ -13099,7 +13114,7 @@
       <c r="D14">
         <v>1352.9</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <f t="shared" si="0"/>
         <v>22.548333333333336</v>
       </c>
@@ -13114,7 +13129,7 @@
       <c r="D15">
         <v>906</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <f t="shared" si="0"/>
         <v>15.1</v>
       </c>
@@ -13129,7 +13144,7 @@
       <c r="D16">
         <v>935.5</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <f t="shared" si="0"/>
         <v>15.591666666666667</v>
       </c>
@@ -13144,7 +13159,7 @@
       <c r="D17">
         <v>915.8</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <f t="shared" si="0"/>
         <v>15.263333333333332</v>
       </c>
@@ -13159,7 +13174,7 @@
       <c r="D18">
         <v>858.3</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <f t="shared" si="0"/>
         <v>14.305</v>
       </c>
@@ -13174,7 +13189,7 @@
       <c r="D19">
         <v>1136.5999999999999</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f t="shared" si="0"/>
         <v>18.943333333333332</v>
       </c>
@@ -13189,7 +13204,7 @@
       <c r="D20">
         <v>2008.9</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <f t="shared" si="0"/>
         <v>33.481666666666669</v>
       </c>
@@ -13204,7 +13219,7 @@
       <c r="D21">
         <v>1197.0999999999999</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <f t="shared" si="0"/>
         <v>19.951666666666664</v>
       </c>
@@ -13219,7 +13234,7 @@
       <c r="D22">
         <v>724.4</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <f t="shared" si="0"/>
         <v>12.073333333333332</v>
       </c>
@@ -13234,7 +13249,7 @@
       <c r="D23">
         <v>1304.0999999999999</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <f t="shared" si="0"/>
         <v>21.734999999999999</v>
       </c>
@@ -13249,7 +13264,7 @@
       <c r="D24">
         <v>1117.4000000000001</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <f t="shared" si="0"/>
         <v>18.623333333333335</v>
       </c>
@@ -13264,7 +13279,7 @@
       <c r="D25">
         <v>611.4</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <f t="shared" si="0"/>
         <v>10.19</v>
       </c>
@@ -13279,7 +13294,7 @@
       <c r="D26">
         <v>614.5</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <f t="shared" si="0"/>
         <v>10.241666666666667</v>
       </c>
@@ -13294,34 +13309,34 @@
       <c r="D27">
         <v>576.79999999999995</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <f t="shared" si="0"/>
         <v>9.6133333333333333</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <f>SUM(B2:B27)</f>
         <v>13239</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <f>AVERAGE(C2:C27)</f>
         <v>41.284615384615378</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <f>AVERAGE(D2:D27)</f>
         <v>983.91923076923081</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="9">
         <f>AVERAGE(E2:E27)</f>
         <v>16.398653846153849</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="E29" s="6"/>
+      <c r="E29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13349,10 +13364,10 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -15499,11 +15514,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D1">
@@ -15520,10 +15535,10 @@
         <f>ROUND(EVERYTHING!G11,0)</f>
         <v>5</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -16328,7 +16343,7 @@
         <v>64</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G98" si="2">COUNTIF(A$2:A$45,F67)</f>
+        <f t="shared" ref="G67:G89" si="2">COUNTIF(A$2:A$45,F67)</f>
         <v>0</v>
       </c>
     </row>
@@ -16562,35 +16577,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="14">
         <f>AVERAGE(A2:A45)</f>
         <v>6.1136363636363633</v>
       </c>
-      <c r="E1" s="11"/>
+      <c r="E1" s="10"/>
       <c r="F1" s="24" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="24"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="13" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="11" t="s">
         <v>26</v>
       </c>
       <c r="T1" s="23" t="s">
@@ -16620,16 +16635,16 @@
         <f t="shared" ref="R2:R27" si="0">ROUND(Q2, 0)</f>
         <v>21</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Y2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="Z2" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -16659,10 +16674,10 @@
         <f t="shared" ref="U3:U42" si="1">COUNTIF(R$2:R$27, T3)</f>
         <v>0</v>
       </c>
-      <c r="Y3" s="6">
+      <c r="Y3" s="5">
         <v>1</v>
       </c>
-      <c r="Z3" s="6">
+      <c r="Z3" s="5">
         <f>G3+U3</f>
         <v>8</v>
       </c>
@@ -16693,10 +16708,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Y4" s="5">
         <v>2</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="Z4" s="5">
         <f t="shared" ref="Z4:Z19" si="3">G4+U4</f>
         <v>3</v>
       </c>
@@ -16727,10 +16742,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Y5" s="5">
         <v>3</v>
       </c>
-      <c r="Z5" s="6">
+      <c r="Z5" s="5">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -16761,10 +16776,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y6" s="6">
+      <c r="Y6" s="5">
         <v>4</v>
       </c>
-      <c r="Z6" s="6">
+      <c r="Z6" s="5">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -16795,10 +16810,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y7" s="6">
+      <c r="Y7" s="5">
         <v>5</v>
       </c>
-      <c r="Z7" s="6">
+      <c r="Z7" s="5">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -16829,10 +16844,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y8" s="6">
+      <c r="Y8" s="5">
         <v>6</v>
       </c>
-      <c r="Z8" s="6">
+      <c r="Z8" s="5">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -16863,10 +16878,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y9" s="6">
+      <c r="Y9" s="5">
         <v>7</v>
       </c>
-      <c r="Z9" s="6">
+      <c r="Z9" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -16897,10 +16912,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y10" s="6">
+      <c r="Y10" s="5">
         <v>8</v>
       </c>
-      <c r="Z10" s="6">
+      <c r="Z10" s="5">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -16931,10 +16946,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y11" s="6">
+      <c r="Y11" s="5">
         <v>9</v>
       </c>
-      <c r="Z11" s="6">
+      <c r="Z11" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -16965,10 +16980,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y12" s="6">
+      <c r="Y12" s="5">
         <v>10</v>
       </c>
-      <c r="Z12" s="6">
+      <c r="Z12" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -16999,10 +17014,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y13" s="6">
+      <c r="Y13" s="5">
         <v>11</v>
       </c>
-      <c r="Z13" s="6">
+      <c r="Z13" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -17033,10 +17048,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y14" s="6">
+      <c r="Y14" s="5">
         <v>12</v>
       </c>
-      <c r="Z14" s="6">
+      <c r="Z14" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -17067,10 +17082,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y15" s="6">
+      <c r="Y15" s="5">
         <v>13</v>
       </c>
-      <c r="Z15" s="6">
+      <c r="Z15" s="5">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -17101,10 +17116,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Y16" s="6">
+      <c r="Y16" s="5">
         <v>14</v>
       </c>
-      <c r="Z16" s="6">
+      <c r="Z16" s="5">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -17135,10 +17150,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y17" s="6">
+      <c r="Y17" s="5">
         <v>15</v>
       </c>
-      <c r="Z17" s="6">
+      <c r="Z17" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -17169,10 +17184,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y18" s="6">
+      <c r="Y18" s="5">
         <v>16</v>
       </c>
-      <c r="Z18" s="6">
+      <c r="Z18" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -17203,10 +17218,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y19" s="6">
+      <c r="Y19" s="5">
         <v>17</v>
       </c>
-      <c r="Z19" s="6">
+      <c r="Z19" s="5">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -17237,17 +17252,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y20" s="6">
+      <c r="Y20" s="5">
         <v>18</v>
       </c>
-      <c r="Z20" s="6">
+      <c r="Z20" s="5">
         <f>G20+U20</f>
         <v>1</v>
       </c>
-      <c r="AF20" s="15" t="s">
+      <c r="AF20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AG20" s="15">
+      <c r="AG20" s="14">
         <v>12.75714</v>
       </c>
     </row>
@@ -17277,10 +17292,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y21" s="6">
+      <c r="Y21" s="5">
         <v>19</v>
       </c>
-      <c r="Z21" s="6">
+      <c r="Z21" s="5">
         <f>G21+U21</f>
         <v>1</v>
       </c>
@@ -17310,10 +17325,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y22" s="6">
+      <c r="Y22" s="5">
         <v>20</v>
       </c>
-      <c r="Z22" s="6">
+      <c r="Z22" s="5">
         <f t="shared" ref="Z22:Z39" si="4">G22+U22</f>
         <v>0</v>
       </c>
@@ -17343,10 +17358,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y23" s="6">
+      <c r="Y23" s="5">
         <v>21</v>
       </c>
-      <c r="Z23" s="6">
+      <c r="Z23" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -17376,10 +17391,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y24" s="6">
+      <c r="Y24" s="5">
         <v>22</v>
       </c>
-      <c r="Z24" s="6">
+      <c r="Z24" s="5">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17409,10 +17424,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y25" s="6">
+      <c r="Y25" s="5">
         <v>23</v>
       </c>
-      <c r="Z25" s="6">
+      <c r="Z25" s="5">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17442,10 +17457,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y26" s="6">
+      <c r="Y26" s="5">
         <v>24</v>
       </c>
-      <c r="Z26" s="6">
+      <c r="Z26" s="5">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17475,10 +17490,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y27" s="6">
+      <c r="Y27" s="5">
         <v>25</v>
       </c>
-      <c r="Z27" s="6">
+      <c r="Z27" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17500,10 +17515,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y28" s="6">
+      <c r="Y28" s="5">
         <v>26</v>
       </c>
-      <c r="Z28" s="6">
+      <c r="Z28" s="5">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17518,10 +17533,10 @@
       <c r="G29">
         <v>0</v>
       </c>
-      <c r="Q29" s="16" t="s">
+      <c r="Q29" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="R29" s="19">
+      <c r="R29" s="18">
         <f>AVERAGE(R2:R27)</f>
         <v>24</v>
       </c>
@@ -17532,10 +17547,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Y29" s="6">
+      <c r="Y29" s="5">
         <v>27</v>
       </c>
-      <c r="Z29" s="6">
+      <c r="Z29" s="5">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -17557,10 +17572,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y30" s="6">
+      <c r="Y30" s="5">
         <v>28</v>
       </c>
-      <c r="Z30" s="6">
+      <c r="Z30" s="5">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17582,10 +17597,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y31" s="6">
+      <c r="Y31" s="5">
         <v>29</v>
       </c>
-      <c r="Z31" s="6">
+      <c r="Z31" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17607,10 +17622,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y32" s="6">
+      <c r="Y32" s="5">
         <v>30</v>
       </c>
-      <c r="Z32" s="6">
+      <c r="Z32" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17632,10 +17647,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y33" s="6">
+      <c r="Y33" s="5">
         <v>31</v>
       </c>
-      <c r="Z33" s="6">
+      <c r="Z33" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17657,10 +17672,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y34" s="6">
+      <c r="Y34" s="5">
         <v>32</v>
       </c>
-      <c r="Z34" s="6">
+      <c r="Z34" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -17682,10 +17697,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y35" s="6">
+      <c r="Y35" s="5">
         <v>33</v>
       </c>
-      <c r="Z35" s="6">
+      <c r="Z35" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17707,10 +17722,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y36" s="6">
+      <c r="Y36" s="5">
         <v>34</v>
       </c>
-      <c r="Z36" s="6">
+      <c r="Z36" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17732,10 +17747,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y37" s="6">
+      <c r="Y37" s="5">
         <v>35</v>
       </c>
-      <c r="Z37" s="6">
+      <c r="Z37" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17757,10 +17772,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y38" s="6">
+      <c r="Y38" s="5">
         <v>36</v>
       </c>
-      <c r="Z38" s="6">
+      <c r="Z38" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17782,10 +17797,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y39" s="6">
+      <c r="Y39" s="5">
         <v>37</v>
       </c>
-      <c r="Z39" s="6">
+      <c r="Z39" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -17801,7 +17816,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y40" s="6">
+      <c r="Y40" s="5">
         <v>38</v>
       </c>
       <c r="Z40">
@@ -17819,7 +17834,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y41" s="6">
+      <c r="Y41" s="5">
         <v>39</v>
       </c>
       <c r="Z41">
@@ -17837,7 +17852,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y42" s="6">
+      <c r="Y42" s="5">
         <v>40</v>
       </c>
       <c r="Z42">
@@ -17878,7 +17893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -17890,74 +17905,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="19">
+      <c r="B1" s="18">
         <v>20.344537819999999</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="21">
+      <c r="F1" s="20">
         <v>0.25</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="18">
         <v>28.818180000000002</v>
       </c>
       <c r="C2" s="25"/>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>0.27331100000000003</v>
       </c>
       <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>6.1135999999999999</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="21">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>12.75</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="15"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
sim is all done except for random draws
</commit_message>
<xml_diff>
--- a/Giant Eagle Data Stuff.xlsx
+++ b/Giant Eagle Data Stuff.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="EVERYTHING" sheetId="1" r:id="rId1"/>
@@ -189,12 +189,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -221,23 +227,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,9 +274,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,8 +286,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,11 +827,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="5891680"/>
-        <c:axId val="176947504"/>
+        <c:axId val="1281819056"/>
+        <c:axId val="1281818512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5891680"/>
+        <c:axId val="1281819056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,7 +929,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="176947504"/>
+        <c:crossAx val="1281818512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -933,7 +938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="176947504"/>
+        <c:axId val="1281818512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1040,7 +1045,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5891680"/>
+        <c:crossAx val="1281819056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1320,11 +1325,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="236706768"/>
-        <c:axId val="236705680"/>
+        <c:axId val="1489718272"/>
+        <c:axId val="1489732960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="236706768"/>
+        <c:axId val="1489718272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1371,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236705680"/>
+        <c:crossAx val="1489732960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1374,7 +1379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236705680"/>
+        <c:axId val="1489732960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236706768"/>
+        <c:crossAx val="1489718272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1514,6 +1519,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1844,11 +1850,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235535312"/>
-        <c:axId val="235534224"/>
+        <c:axId val="1110341952"/>
+        <c:axId val="1110344672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235535312"/>
+        <c:axId val="1110341952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1890,7 +1896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235534224"/>
+        <c:crossAx val="1110344672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1898,7 +1904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235534224"/>
+        <c:axId val="1110344672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235535312"/>
+        <c:crossAx val="1110341952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2038,6 +2044,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2164,11 +2171,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235532048"/>
-        <c:axId val="235544016"/>
+        <c:axId val="1335525824"/>
+        <c:axId val="1335539424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235532048"/>
+        <c:axId val="1335525824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2210,7 +2217,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235544016"/>
+        <c:crossAx val="1335539424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2218,7 +2225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235544016"/>
+        <c:axId val="1335539424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2269,7 +2276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235532048"/>
+        <c:crossAx val="1335525824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2358,6 +2365,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2547,11 +2555,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235539120"/>
-        <c:axId val="235545104"/>
+        <c:axId val="1335533440"/>
+        <c:axId val="1335531808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235539120"/>
+        <c:axId val="1335533440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2593,7 +2601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235545104"/>
+        <c:crossAx val="1335531808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2601,7 +2609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235545104"/>
+        <c:axId val="1335531808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2652,7 +2660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235539120"/>
+        <c:crossAx val="1335533440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2741,6 +2749,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2930,11 +2939,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235531504"/>
-        <c:axId val="235539664"/>
+        <c:axId val="1335532352"/>
+        <c:axId val="1335524736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235531504"/>
+        <c:axId val="1335532352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2976,7 +2985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235539664"/>
+        <c:crossAx val="1335524736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2984,7 +2993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235539664"/>
+        <c:axId val="1335524736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3035,7 +3044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235531504"/>
+        <c:crossAx val="1335532352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3605,11 +3614,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235540752"/>
-        <c:axId val="235536400"/>
+        <c:axId val="1050482880"/>
+        <c:axId val="1050487232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235540752"/>
+        <c:axId val="1050482880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3707,7 +3716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235536400"/>
+        <c:crossAx val="1050487232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3716,7 +3725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235536400"/>
+        <c:axId val="1050487232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3823,7 +3832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235540752"/>
+        <c:crossAx val="1050482880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4244,11 +4253,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235541296"/>
-        <c:axId val="235533680"/>
+        <c:axId val="1281809264"/>
+        <c:axId val="1281809808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235541296"/>
+        <c:axId val="1281809264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4290,7 +4299,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235533680"/>
+        <c:crossAx val="1281809808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4298,7 +4307,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235533680"/>
+        <c:axId val="1281809808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4349,7 +4358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235541296"/>
+        <c:crossAx val="1281809264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4438,6 +4447,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4564,11 +4574,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="235538576"/>
-        <c:axId val="235538032"/>
+        <c:axId val="1050486688"/>
+        <c:axId val="1050485600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235538576"/>
+        <c:axId val="1050486688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4610,7 +4620,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235538032"/>
+        <c:crossAx val="1050485600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4618,7 +4628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235538032"/>
+        <c:axId val="1050485600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4669,7 +4679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235538576"/>
+        <c:crossAx val="1050486688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4758,6 +4768,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4947,11 +4958,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="236692080"/>
-        <c:axId val="236696432"/>
+        <c:axId val="1489719904"/>
+        <c:axId val="1489728064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="236692080"/>
+        <c:axId val="1489719904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4993,7 +5004,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236696432"/>
+        <c:crossAx val="1489728064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5001,7 +5012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236696432"/>
+        <c:axId val="1489728064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5052,7 +5063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236692080"/>
+        <c:crossAx val="1489719904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11124,10 +11135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J249"/>
+  <dimension ref="A1:J239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E249" sqref="A249:E249"/>
+    <sheetView topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -11145,7 +11156,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -11161,10 +11172,10 @@
         <v>8</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>28</v>
       </c>
     </row>
@@ -11174,7 +11185,7 @@
       </c>
       <c r="B2">
         <f>AVERAGE(A2:A239)</f>
-        <v>22.483193277310924</v>
+        <v>20.344537815126049</v>
       </c>
       <c r="D2" s="2">
         <v>6</v>
@@ -11186,11 +11197,11 @@
         <f>E2/D2</f>
         <v>11.333333333333334</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <f>AVERAGE(E2:E45)</f>
         <v>115.5</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="6">
         <f>AVERAGE(G2:G45)</f>
         <v>28.765203045617486</v>
       </c>
@@ -11212,7 +11223,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
@@ -11355,7 +11366,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -11371,7 +11382,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2">
         <v>5</v>
@@ -11387,7 +11398,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2">
         <v>14</v>
@@ -11403,7 +11414,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2">
         <v>4</v>
@@ -11499,7 +11510,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -11515,7 +11526,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
@@ -11531,7 +11542,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -11547,7 +11558,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2">
         <v>4</v>
@@ -11563,7 +11574,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
@@ -11579,7 +11590,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27" s="2">
         <v>5</v>
@@ -11613,7 +11624,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="2">
         <v>5</v>
@@ -11629,7 +11640,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" s="2">
         <v>2</v>
@@ -11645,7 +11656,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
@@ -11661,7 +11672,7 @@
     </row>
     <row r="32" spans="1:7" ht="12.75">
       <c r="A32" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2">
         <v>5</v>
@@ -11677,7 +11688,7 @@
     </row>
     <row r="33" spans="1:7" ht="12.75">
       <c r="A33" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2">
         <v>6</v>
@@ -11695,7 +11706,7 @@
     </row>
     <row r="34" spans="1:7" ht="12.75">
       <c r="A34" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D34" s="2">
         <v>9</v>
@@ -11711,7 +11722,7 @@
     </row>
     <row r="35" spans="1:7" ht="12.75">
       <c r="A35" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35" s="2">
         <v>3</v>
@@ -11727,7 +11738,7 @@
     </row>
     <row r="36" spans="1:7" ht="12.75">
       <c r="A36" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D36" s="2">
         <v>12</v>
@@ -11825,7 +11836,7 @@
     </row>
     <row r="42" spans="1:7" ht="12.75">
       <c r="A42" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
@@ -11841,7 +11852,7 @@
     </row>
     <row r="43" spans="1:7" ht="12.75">
       <c r="A43" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D43" s="2">
         <v>11</v>
@@ -11857,7 +11868,7 @@
     </row>
     <row r="44" spans="1:7" ht="12.75">
       <c r="A44" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D44" s="2">
         <v>8</v>
@@ -11875,7 +11886,7 @@
     </row>
     <row r="45" spans="1:7" ht="12.75">
       <c r="A45" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D45" s="2">
         <v>2</v>
@@ -11891,768 +11902,754 @@
     </row>
     <row r="46" spans="1:7" ht="12.75">
       <c r="A46" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="12.75">
       <c r="A47" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="12.75">
       <c r="A48" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="12.75">
       <c r="A49" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="12.75">
       <c r="A50" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="12.75">
       <c r="A51" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="12.75">
       <c r="A52" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="12.75">
       <c r="A53" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="12.75">
       <c r="A54" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="12.75">
       <c r="A55" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="12.75">
       <c r="A56" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="12.75">
       <c r="A57" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="12.75">
       <c r="A58" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="12.75">
       <c r="A59" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="12.75">
       <c r="A60" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="12.75">
       <c r="A61" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="12.75">
       <c r="A62" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="12.75">
       <c r="A63" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="12.75">
       <c r="A64" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="12.75">
       <c r="A65" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="12.75">
       <c r="A66" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="12.75">
       <c r="A67" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="12.75">
       <c r="A68" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="12.75">
       <c r="A69" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="12.75">
       <c r="A70" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="12.75">
       <c r="A71" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="12.75">
       <c r="A72" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="12.75">
       <c r="A73" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="12.75">
       <c r="A74" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="12.75">
       <c r="A75" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="12.75">
       <c r="A76" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="12.75">
       <c r="A77" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="12.75">
       <c r="A78" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="12.75">
       <c r="A79" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="12.75">
       <c r="A80" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="12.75">
+      <c r="A81" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="12.75">
+      <c r="A82" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="12.75">
+      <c r="A83" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="12.75">
+      <c r="A84" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="12.75">
+      <c r="A85" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="12.75">
+      <c r="A86" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="12.75">
+      <c r="A87" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="12.75">
+      <c r="A88" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="12.75">
+      <c r="A89" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="12.75">
+      <c r="A90" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="12.75">
+      <c r="A91" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="12.75">
+      <c r="A92" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="12.75">
+      <c r="A93" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="12.75">
+      <c r="A94" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="12.75">
+      <c r="A95" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="12.75">
-      <c r="A81" s="2">
+    <row r="96" spans="1:1" ht="12.75">
+      <c r="A96" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" ht="12.75">
-      <c r="A82" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="12.75">
-      <c r="A83" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="12.75">
-      <c r="A84" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="12.75">
-      <c r="A85" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="12.75">
-      <c r="A86" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="12.75">
-      <c r="A87" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="12.75">
-      <c r="A88" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="12.75">
-      <c r="A89" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="12.75">
-      <c r="A90" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="12.75">
-      <c r="A91" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="12.75">
-      <c r="A92" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="12.75">
-      <c r="A93" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="12.75">
-      <c r="A94" s="2">
-        <v>11</v>
-      </c>
-      <c r="D94" s="26"/>
-    </row>
-    <row r="95" spans="1:4" ht="12.75">
-      <c r="A95" s="2">
-        <v>12</v>
-      </c>
-      <c r="D95" s="26"/>
-    </row>
-    <row r="96" spans="1:4" ht="12.75">
-      <c r="A96" s="2">
-        <v>12</v>
-      </c>
-      <c r="D96" s="26"/>
     </row>
     <row r="97" spans="1:4" ht="12.75">
       <c r="A97" s="2">
-        <v>12</v>
-      </c>
-      <c r="D97" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="98" spans="1:4" ht="12.75">
       <c r="A98" s="2">
-        <v>12</v>
-      </c>
-      <c r="D98" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="99" spans="1:4" ht="12.75">
       <c r="A99" s="2">
-        <v>12</v>
-      </c>
-      <c r="D99" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="100" spans="1:4" ht="12.75">
       <c r="A100" s="2">
-        <v>13</v>
-      </c>
-      <c r="D100" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="101" spans="1:4" ht="12.75">
       <c r="A101" s="2">
-        <v>13</v>
-      </c>
-      <c r="D101" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="102" spans="1:4" ht="12.75">
       <c r="A102" s="2">
-        <v>13</v>
-      </c>
-      <c r="D102" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="103" spans="1:4" ht="14.25">
       <c r="A103" s="2">
-        <v>13</v>
-      </c>
-      <c r="D103" s="27"/>
+        <v>10</v>
+      </c>
+      <c r="D103" s="3"/>
     </row>
     <row r="104" spans="1:4" ht="12.75">
       <c r="A104" s="2">
-        <v>13</v>
-      </c>
-      <c r="D104" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="105" spans="1:4" ht="14.25">
       <c r="A105" s="2">
-        <v>13</v>
-      </c>
-      <c r="D105" s="27"/>
+        <v>10</v>
+      </c>
+      <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" ht="12.75">
       <c r="A106" s="2">
-        <v>13</v>
-      </c>
-      <c r="D106" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="107" spans="1:4" ht="12.75">
       <c r="A107" s="2">
-        <v>14</v>
-      </c>
-      <c r="D107" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="108" spans="1:4" ht="12.75">
       <c r="A108" s="2">
-        <v>14</v>
-      </c>
-      <c r="D108" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="12.75">
       <c r="A109" s="2">
-        <v>14</v>
-      </c>
-      <c r="D109" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="110" spans="1:4" ht="12.75">
       <c r="A110" s="2">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="12.75">
       <c r="A111" s="2">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="12.75">
       <c r="A112" s="2">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="12.75">
       <c r="A113" s="2">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="12.75">
       <c r="A114" s="2">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="12.75">
       <c r="A115" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="12.75">
       <c r="A116" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="12.75">
       <c r="A117" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="12.75">
       <c r="A118" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="12.75">
       <c r="A119" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="12.75">
       <c r="A120" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="12.75">
       <c r="A121" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="12.75">
       <c r="A122" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="12.75">
       <c r="A123" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="12.75">
       <c r="A124" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="12.75">
       <c r="A125" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="12.75">
       <c r="A126" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="12.75">
       <c r="A127" s="2">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="12.75">
       <c r="A128" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="12.75">
       <c r="A129" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="12.75">
       <c r="A130" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="12.75">
       <c r="A131" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="12.75">
       <c r="A132" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="12.75">
       <c r="A133" s="2">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="12.75">
       <c r="A134" s="2">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="12.75">
       <c r="A135" s="2">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="12.75">
       <c r="A136" s="2">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="12.75">
       <c r="A137" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="12.75">
       <c r="A138" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="12.75">
       <c r="A139" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="12.75">
       <c r="A140" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="12.75">
       <c r="A141" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="12.75">
-      <c r="A142" s="5">
-        <v>21</v>
+      <c r="A142" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="12.75">
-      <c r="A143" s="5">
-        <v>21</v>
+      <c r="A143" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="12.75">
       <c r="A144" s="2">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="12.75">
       <c r="A145" s="2">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="12.75">
       <c r="A146" s="2">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="12.75">
-      <c r="A147" s="5">
-        <v>22</v>
+      <c r="A147" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="12.75">
-      <c r="A148" s="5">
-        <v>22</v>
+      <c r="A148" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="12.75">
       <c r="A149" s="2">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="12.75">
       <c r="A150" s="2">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="12.75">
-      <c r="A151" s="5">
-        <v>23</v>
+      <c r="A151" s="2">
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="12.75">
       <c r="A152" s="2">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="12.75">
-      <c r="A153" s="5">
-        <v>24</v>
+      <c r="A153" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="12.75">
-      <c r="A154" s="5">
-        <v>24</v>
+      <c r="A154" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="12.75">
       <c r="A155" s="2">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="12.75">
-      <c r="A156" s="5">
-        <v>25</v>
+      <c r="A156" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="12.75">
       <c r="A157" s="2">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="12.75">
       <c r="A158" s="2">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="12.75">
-      <c r="A159" s="5">
-        <v>26</v>
+      <c r="A159" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="12.75">
       <c r="A160" s="2">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="12.75">
-      <c r="A161" s="5">
-        <v>27</v>
+      <c r="A161" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="12.75">
-      <c r="A162" s="5">
-        <v>27</v>
+      <c r="A162" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="12.75">
-      <c r="A163" s="5">
-        <v>27</v>
+      <c r="A163" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="12.75">
       <c r="A164" s="2">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="12.75">
       <c r="A165" s="2">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="12.75">
       <c r="A166" s="2">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="12.75">
       <c r="A167" s="2">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="12.75">
-      <c r="A168" s="5">
-        <v>28</v>
+      <c r="A168" s="2">
+        <v>21</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="12.75">
-      <c r="A169" s="5">
-        <v>28</v>
+      <c r="A169" s="2">
+        <v>21</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="12.75">
       <c r="A170" s="2">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="12.75">
       <c r="A171" s="2">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="12.75">
-      <c r="A172" s="5">
-        <v>29</v>
+      <c r="A172" s="2">
+        <v>23</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="12.75">
       <c r="A173" s="2">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="12.75">
-      <c r="A174" s="5">
-        <v>30</v>
+      <c r="A174" s="2">
+        <v>25</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="12.75">
-      <c r="A175" s="5">
-        <v>30</v>
+      <c r="A175" s="2">
+        <v>25</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="12.75">
       <c r="A176" s="2">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="12.75">
       <c r="A177" s="2">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="12.75">
       <c r="A178" s="2">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="12.75">
-      <c r="A179" s="5">
-        <v>31</v>
+      <c r="A179" s="2">
+        <v>27</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="12.75">
       <c r="A180" s="2">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="12.75">
       <c r="A181" s="2">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="12.75">
       <c r="A182" s="2">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="12.75">
-      <c r="A183" s="5">
-        <v>32</v>
+      <c r="A183" s="2">
+        <v>29</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="12.75">
       <c r="A184" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="185" spans="1:1" ht="12.75">
       <c r="A185" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="186" spans="1:1" ht="12.75">
-      <c r="A186" s="5">
-        <v>33</v>
+      <c r="A186" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="187" spans="1:1" ht="12.75">
       <c r="A187" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="12.75">
       <c r="A188" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="189" spans="1:1" ht="12.75">
-      <c r="A189" s="5">
-        <v>34</v>
+      <c r="A189" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="190" spans="1:1" ht="12.75">
-      <c r="A190" s="5">
-        <v>35</v>
+      <c r="A190" s="2">
+        <v>32</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="12.75">
       <c r="A191" s="2">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="12.75">
       <c r="A192" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" ht="12.75">
+      <c r="A193" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" ht="12.75">
+      <c r="A194" s="2">
         <v>35</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" ht="12.75">
-      <c r="A193" s="5">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" ht="12.75">
-      <c r="A194" s="5">
-        <v>37</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="12.75">
       <c r="A195" s="2">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="12.75">
@@ -12666,8 +12663,8 @@
       </c>
     </row>
     <row r="198" spans="1:1" ht="12.75">
-      <c r="A198" s="5">
-        <v>38</v>
+      <c r="A198" s="2">
+        <v>37</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="12.75">
@@ -12681,83 +12678,83 @@
       </c>
     </row>
     <row r="201" spans="1:1" ht="12.75">
-      <c r="A201" s="5">
+      <c r="A201" s="2">
         <v>39</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="12.75">
-      <c r="A202" s="5">
-        <v>39</v>
+      <c r="A202" s="2">
+        <v>40</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="12.75">
       <c r="A203" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="204" spans="1:1" ht="12.75">
-      <c r="A204" s="5">
-        <v>40</v>
+      <c r="A204" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="205" spans="1:1" ht="12.75">
-      <c r="A205" s="5">
-        <v>40</v>
+      <c r="A205" s="2">
+        <v>43</v>
       </c>
     </row>
     <row r="206" spans="1:1" ht="12.75">
-      <c r="A206" s="5">
-        <v>40</v>
+      <c r="A206" s="2">
+        <v>44</v>
       </c>
     </row>
     <row r="207" spans="1:1" ht="12.75">
       <c r="A207" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="208" spans="1:1" ht="12.75">
       <c r="A208" s="2">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="12.75">
       <c r="A209" s="2">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="12.75">
       <c r="A210" s="2">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="211" spans="1:1" ht="12.75">
       <c r="A211" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="212" spans="1:1" ht="12.75">
       <c r="A212" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="12.75">
       <c r="A213" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="12.75">
       <c r="A214" s="2">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="12.75">
       <c r="A215" s="2">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="12.75">
       <c r="A216" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="12.75">
@@ -12777,7 +12774,7 @@
     </row>
     <row r="220" spans="1:1" ht="12.75">
       <c r="A220" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="221" spans="1:1" ht="12.75">
@@ -12787,72 +12784,72 @@
     </row>
     <row r="222" spans="1:1" ht="12.75">
       <c r="A222" s="2">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="223" spans="1:1" ht="12.75">
       <c r="A223" s="2">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="224" spans="1:1" ht="12.75">
       <c r="A224" s="2">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="225" spans="1:1" ht="12.75">
-      <c r="A225" s="5">
-        <v>70</v>
+      <c r="A225" s="2">
+        <v>58</v>
       </c>
     </row>
     <row r="226" spans="1:1" ht="12.75">
-      <c r="A226" s="5">
-        <v>70</v>
+      <c r="A226" s="2">
+        <v>58</v>
       </c>
     </row>
     <row r="227" spans="1:1" ht="12.75">
       <c r="A227" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" ht="12.75">
+      <c r="A228" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="228" spans="1:1" ht="12.75">
-      <c r="A228" s="5">
-        <v>73</v>
-      </c>
-    </row>
     <row r="229" spans="1:1" ht="12.75">
-      <c r="A229" s="5">
-        <v>75</v>
+      <c r="A229" s="2">
+        <v>76</v>
       </c>
     </row>
     <row r="230" spans="1:1" ht="12.75">
       <c r="A230" s="2">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="231" spans="1:1" ht="12.75">
-      <c r="A231" s="5">
-        <v>77</v>
+      <c r="A231" s="2">
+        <v>79</v>
       </c>
     </row>
     <row r="232" spans="1:1" ht="12.75">
       <c r="A232" s="2">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="233" spans="1:1" ht="12.75">
       <c r="A233" s="2">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="234" spans="1:1" ht="12.75">
-      <c r="A234" s="5">
-        <v>80</v>
+      <c r="A234" s="2">
+        <v>85</v>
       </c>
     </row>
     <row r="235" spans="1:1" ht="12.75">
       <c r="A235" s="2">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="236" spans="1:1" ht="12.75">
@@ -12867,7 +12864,7 @@
     </row>
     <row r="238" spans="1:1" ht="12.75">
       <c r="A238" s="2">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="239" spans="1:1" ht="12.75">
@@ -12875,19 +12872,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="240" spans="1:1" ht="12.75"/>
-    <row r="241" spans="1:4" ht="12.75"/>
-    <row r="242" spans="1:4" ht="12.75"/>
-    <row r="243" spans="1:4" ht="12.75"/>
-    <row r="244" spans="1:4" ht="12.75"/>
-    <row r="249" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A249" s="5"/>
-      <c r="D249" s="5"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:B239">
-    <sortCondition ref="A2"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12911,16 +12896,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -12934,7 +12919,7 @@
       <c r="D2">
         <v>974.3</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="8">
         <f>D2/60</f>
         <v>16.238333333333333</v>
       </c>
@@ -12949,7 +12934,7 @@
       <c r="D3">
         <v>470.3</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="8">
         <f t="shared" ref="E3:E27" si="0">D3/60</f>
         <v>7.8383333333333338</v>
       </c>
@@ -12961,10 +12946,10 @@
       <c r="C4">
         <v>34.200000000000003</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>741.2</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="8">
         <f t="shared" si="0"/>
         <v>12.353333333333333</v>
       </c>
@@ -12979,7 +12964,7 @@
       <c r="D5">
         <v>1046.2</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="8">
         <f t="shared" si="0"/>
         <v>17.436666666666667</v>
       </c>
@@ -12994,7 +12979,7 @@
       <c r="D6">
         <v>1120.4000000000001</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
         <v>18.673333333333336</v>
       </c>
@@ -13009,7 +12994,7 @@
       <c r="D7">
         <v>952.3</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
         <v>15.871666666666666</v>
       </c>
@@ -13024,7 +13009,7 @@
       <c r="D8">
         <v>1309.9000000000001</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>21.831666666666667</v>
       </c>
@@ -13039,7 +13024,7 @@
       <c r="D9">
         <v>605</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>10.083333333333334</v>
       </c>
@@ -13054,7 +13039,7 @@
       <c r="D10">
         <v>1077.3</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
         <v>17.954999999999998</v>
       </c>
@@ -13069,7 +13054,7 @@
       <c r="D11">
         <v>1076.2</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>17.936666666666667</v>
       </c>
@@ -13084,7 +13069,7 @@
       <c r="D12">
         <v>976.2</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
         <v>16.27</v>
       </c>
@@ -13099,7 +13084,7 @@
       <c r="D13">
         <v>972.9</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
         <v>16.215</v>
       </c>
@@ -13114,7 +13099,7 @@
       <c r="D14">
         <v>1352.9</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>22.548333333333336</v>
       </c>
@@ -13129,7 +13114,7 @@
       <c r="D15">
         <v>906</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
         <v>15.1</v>
       </c>
@@ -13144,7 +13129,7 @@
       <c r="D16">
         <v>935.5</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="8">
         <f t="shared" si="0"/>
         <v>15.591666666666667</v>
       </c>
@@ -13159,7 +13144,7 @@
       <c r="D17">
         <v>915.8</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="8">
         <f t="shared" si="0"/>
         <v>15.263333333333332</v>
       </c>
@@ -13174,7 +13159,7 @@
       <c r="D18">
         <v>858.3</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="8">
         <f t="shared" si="0"/>
         <v>14.305</v>
       </c>
@@ -13189,7 +13174,7 @@
       <c r="D19">
         <v>1136.5999999999999</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="8">
         <f t="shared" si="0"/>
         <v>18.943333333333332</v>
       </c>
@@ -13204,7 +13189,7 @@
       <c r="D20">
         <v>2008.9</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="8">
         <f t="shared" si="0"/>
         <v>33.481666666666669</v>
       </c>
@@ -13219,7 +13204,7 @@
       <c r="D21">
         <v>1197.0999999999999</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="8">
         <f t="shared" si="0"/>
         <v>19.951666666666664</v>
       </c>
@@ -13234,7 +13219,7 @@
       <c r="D22">
         <v>724.4</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="8">
         <f t="shared" si="0"/>
         <v>12.073333333333332</v>
       </c>
@@ -13249,7 +13234,7 @@
       <c r="D23">
         <v>1304.0999999999999</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <f t="shared" si="0"/>
         <v>21.734999999999999</v>
       </c>
@@ -13264,7 +13249,7 @@
       <c r="D24">
         <v>1117.4000000000001</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="8">
         <f t="shared" si="0"/>
         <v>18.623333333333335</v>
       </c>
@@ -13279,7 +13264,7 @@
       <c r="D25">
         <v>611.4</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="8">
         <f t="shared" si="0"/>
         <v>10.19</v>
       </c>
@@ -13294,7 +13279,7 @@
       <c r="D26">
         <v>614.5</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="8">
         <f t="shared" si="0"/>
         <v>10.241666666666667</v>
       </c>
@@ -13309,34 +13294,34 @@
       <c r="D27">
         <v>576.79999999999995</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="8">
         <f t="shared" si="0"/>
         <v>9.6133333333333333</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="5">
         <f>SUM(B2:B27)</f>
         <v>13239</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="5">
         <f>AVERAGE(C2:C27)</f>
         <v>41.284615384615378</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="5">
         <f>AVERAGE(D2:D27)</f>
         <v>983.91923076923081</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="10">
         <f>AVERAGE(E2:E27)</f>
         <v>16.398653846153849</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="E29" s="5"/>
+      <c r="E29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13364,10 +13349,10 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -15514,11 +15499,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D1">
@@ -15535,10 +15520,10 @@
         <f>ROUND(EVERYTHING!G11,0)</f>
         <v>5</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
@@ -16343,7 +16328,7 @@
         <v>64</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G89" si="2">COUNTIF(A$2:A$45,F67)</f>
+        <f t="shared" ref="G67:G98" si="2">COUNTIF(A$2:A$45,F67)</f>
         <v>0</v>
       </c>
     </row>
@@ -16577,35 +16562,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="15">
         <f>AVERAGE(A2:A45)</f>
         <v>6.1136363636363633</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="24" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="24"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="12" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="12" t="s">
         <v>26</v>
       </c>
       <c r="T1" s="23" t="s">
@@ -16635,16 +16620,16 @@
         <f t="shared" ref="R2:R27" si="0">ROUND(Q2, 0)</f>
         <v>21</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="T2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="U2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Y2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="Z2" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -16674,10 +16659,10 @@
         <f t="shared" ref="U3:U42" si="1">COUNTIF(R$2:R$27, T3)</f>
         <v>0</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Y3" s="6">
         <v>1</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="Z3" s="6">
         <f>G3+U3</f>
         <v>8</v>
       </c>
@@ -16708,10 +16693,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="6">
         <v>2</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="Z4" s="6">
         <f t="shared" ref="Z4:Z19" si="3">G4+U4</f>
         <v>3</v>
       </c>
@@ -16742,10 +16727,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y5" s="5">
+      <c r="Y5" s="6">
         <v>3</v>
       </c>
-      <c r="Z5" s="5">
+      <c r="Z5" s="6">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -16776,10 +16761,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y6" s="5">
+      <c r="Y6" s="6">
         <v>4</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Z6" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -16810,10 +16795,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y7" s="5">
+      <c r="Y7" s="6">
         <v>5</v>
       </c>
-      <c r="Z7" s="5">
+      <c r="Z7" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -16844,10 +16829,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y8" s="5">
+      <c r="Y8" s="6">
         <v>6</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="Z8" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -16878,10 +16863,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y9" s="5">
+      <c r="Y9" s="6">
         <v>7</v>
       </c>
-      <c r="Z9" s="5">
+      <c r="Z9" s="6">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -16912,10 +16897,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y10" s="5">
+      <c r="Y10" s="6">
         <v>8</v>
       </c>
-      <c r="Z10" s="5">
+      <c r="Z10" s="6">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -16946,10 +16931,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y11" s="5">
+      <c r="Y11" s="6">
         <v>9</v>
       </c>
-      <c r="Z11" s="5">
+      <c r="Z11" s="6">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -16980,10 +16965,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="Y12" s="6">
         <v>10</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z12" s="6">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -17014,10 +16999,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y13" s="5">
+      <c r="Y13" s="6">
         <v>11</v>
       </c>
-      <c r="Z13" s="5">
+      <c r="Z13" s="6">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -17048,10 +17033,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y14" s="5">
+      <c r="Y14" s="6">
         <v>12</v>
       </c>
-      <c r="Z14" s="5">
+      <c r="Z14" s="6">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -17082,10 +17067,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y15" s="5">
+      <c r="Y15" s="6">
         <v>13</v>
       </c>
-      <c r="Z15" s="5">
+      <c r="Z15" s="6">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -17116,10 +17101,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Y16" s="5">
+      <c r="Y16" s="6">
         <v>14</v>
       </c>
-      <c r="Z16" s="5">
+      <c r="Z16" s="6">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -17150,10 +17135,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y17" s="5">
+      <c r="Y17" s="6">
         <v>15</v>
       </c>
-      <c r="Z17" s="5">
+      <c r="Z17" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -17184,10 +17169,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y18" s="5">
+      <c r="Y18" s="6">
         <v>16</v>
       </c>
-      <c r="Z18" s="5">
+      <c r="Z18" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -17218,10 +17203,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y19" s="5">
+      <c r="Y19" s="6">
         <v>17</v>
       </c>
-      <c r="Z19" s="5">
+      <c r="Z19" s="6">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -17252,17 +17237,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y20" s="5">
+      <c r="Y20" s="6">
         <v>18</v>
       </c>
-      <c r="Z20" s="5">
+      <c r="Z20" s="6">
         <f>G20+U20</f>
         <v>1</v>
       </c>
-      <c r="AF20" s="14" t="s">
+      <c r="AF20" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AG20" s="14">
+      <c r="AG20" s="15">
         <v>12.75714</v>
       </c>
     </row>
@@ -17292,10 +17277,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y21" s="5">
+      <c r="Y21" s="6">
         <v>19</v>
       </c>
-      <c r="Z21" s="5">
+      <c r="Z21" s="6">
         <f>G21+U21</f>
         <v>1</v>
       </c>
@@ -17325,10 +17310,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y22" s="5">
+      <c r="Y22" s="6">
         <v>20</v>
       </c>
-      <c r="Z22" s="5">
+      <c r="Z22" s="6">
         <f t="shared" ref="Z22:Z39" si="4">G22+U22</f>
         <v>0</v>
       </c>
@@ -17358,10 +17343,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y23" s="5">
+      <c r="Y23" s="6">
         <v>21</v>
       </c>
-      <c r="Z23" s="5">
+      <c r="Z23" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -17391,10 +17376,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y24" s="5">
+      <c r="Y24" s="6">
         <v>22</v>
       </c>
-      <c r="Z24" s="5">
+      <c r="Z24" s="6">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17424,10 +17409,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y25" s="5">
+      <c r="Y25" s="6">
         <v>23</v>
       </c>
-      <c r="Z25" s="5">
+      <c r="Z25" s="6">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17457,10 +17442,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y26" s="5">
+      <c r="Y26" s="6">
         <v>24</v>
       </c>
-      <c r="Z26" s="5">
+      <c r="Z26" s="6">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17490,10 +17475,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y27" s="5">
+      <c r="Y27" s="6">
         <v>25</v>
       </c>
-      <c r="Z27" s="5">
+      <c r="Z27" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17515,10 +17500,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y28" s="5">
+      <c r="Y28" s="6">
         <v>26</v>
       </c>
-      <c r="Z28" s="5">
+      <c r="Z28" s="6">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17533,10 +17518,10 @@
       <c r="G29">
         <v>0</v>
       </c>
-      <c r="Q29" s="15" t="s">
+      <c r="Q29" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="R29" s="18">
+      <c r="R29" s="19">
         <f>AVERAGE(R2:R27)</f>
         <v>24</v>
       </c>
@@ -17547,10 +17532,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Y29" s="5">
+      <c r="Y29" s="6">
         <v>27</v>
       </c>
-      <c r="Z29" s="5">
+      <c r="Z29" s="6">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -17572,10 +17557,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="Y30" s="5">
+      <c r="Y30" s="6">
         <v>28</v>
       </c>
-      <c r="Z30" s="5">
+      <c r="Z30" s="6">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
@@ -17597,10 +17582,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y31" s="5">
+      <c r="Y31" s="6">
         <v>29</v>
       </c>
-      <c r="Z31" s="5">
+      <c r="Z31" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17622,10 +17607,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y32" s="5">
+      <c r="Y32" s="6">
         <v>30</v>
       </c>
-      <c r="Z32" s="5">
+      <c r="Z32" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17647,10 +17632,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y33" s="5">
+      <c r="Y33" s="6">
         <v>31</v>
       </c>
-      <c r="Z33" s="5">
+      <c r="Z33" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17672,10 +17657,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y34" s="5">
+      <c r="Y34" s="6">
         <v>32</v>
       </c>
-      <c r="Z34" s="5">
+      <c r="Z34" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -17697,10 +17682,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y35" s="5">
+      <c r="Y35" s="6">
         <v>33</v>
       </c>
-      <c r="Z35" s="5">
+      <c r="Z35" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17722,10 +17707,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y36" s="5">
+      <c r="Y36" s="6">
         <v>34</v>
       </c>
-      <c r="Z36" s="5">
+      <c r="Z36" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17747,10 +17732,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y37" s="5">
+      <c r="Y37" s="6">
         <v>35</v>
       </c>
-      <c r="Z37" s="5">
+      <c r="Z37" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17772,10 +17757,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y38" s="5">
+      <c r="Y38" s="6">
         <v>36</v>
       </c>
-      <c r="Z38" s="5">
+      <c r="Z38" s="6">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -17797,10 +17782,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y39" s="5">
+      <c r="Y39" s="6">
         <v>37</v>
       </c>
-      <c r="Z39" s="5">
+      <c r="Z39" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -17816,7 +17801,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y40" s="5">
+      <c r="Y40" s="6">
         <v>38</v>
       </c>
       <c r="Z40">
@@ -17834,7 +17819,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y41" s="5">
+      <c r="Y41" s="6">
         <v>39</v>
       </c>
       <c r="Z41">
@@ -17852,7 +17837,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y42" s="5">
+      <c r="Y42" s="6">
         <v>40</v>
       </c>
       <c r="Z42">
@@ -17893,7 +17878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -17905,74 +17890,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="18">
+      <c r="B1" s="19">
         <v>20.344537819999999</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="20">
+      <c r="F1" s="21">
         <v>0.25</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="19">
         <v>28.818180000000002</v>
       </c>
       <c r="C2" s="25"/>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="21">
         <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="19">
         <v>0.27331100000000003</v>
       </c>
       <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="19">
         <v>6.1135999999999999</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="26">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="19">
         <v>12.75</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="14"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Technically finished, still has bugs
</commit_message>
<xml_diff>
--- a/Giant Eagle Data Stuff.xlsx
+++ b/Giant Eagle Data Stuff.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EVERYTHING" sheetId="1" r:id="rId1"/>
     <sheet name="Cashier Data" sheetId="5" r:id="rId2"/>
     <sheet name="Arrivals" sheetId="2" r:id="rId3"/>
-    <sheet name="Service Time Per Item" sheetId="4" r:id="rId4"/>
+    <sheet name="Self-Check Time Per Item" sheetId="4" r:id="rId4"/>
     <sheet name="Items Per Customer" sheetId="3" r:id="rId5"/>
     <sheet name="Important Statistics" sheetId="6" r:id="rId6"/>
     <sheet name="Graphs" sheetId="7" r:id="rId7"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Time Between Arrivals</t>
   </si>
@@ -143,13 +143,23 @@
   <si>
     <t>Avg Self-Check Service Time/Item:</t>
   </si>
+  <si>
+    <t>Std. Dev</t>
+  </si>
+  <si>
+    <t>Std.Dev:</t>
+  </si>
+  <si>
+    <t>Std. Dev:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -160,6 +170,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -218,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,6 +280,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -342,7 +357,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -819,11 +833,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1426994384"/>
-        <c:axId val="-1426998736"/>
+        <c:axId val="-1725583264"/>
+        <c:axId val="-1725569664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1426994384"/>
+        <c:axId val="-1725583264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +869,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -921,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1426998736"/>
+        <c:crossAx val="-1725569664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -930,7 +943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1426998736"/>
+        <c:axId val="-1725569664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -976,7 +989,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1037,7 +1049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1426994384"/>
+        <c:crossAx val="-1725583264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1222,16 +1234,16 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
@@ -1316,11 +1328,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1372336496"/>
-        <c:axId val="-1372321808"/>
+        <c:axId val="-1962262608"/>
+        <c:axId val="-1962260976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1372336496"/>
+        <c:axId val="-1962262608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1374,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1372321808"/>
+        <c:crossAx val="-1962260976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1370,7 +1382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1372321808"/>
+        <c:axId val="-1962260976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1421,7 +1433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1372336496"/>
+        <c:crossAx val="-1962262608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1562,7 +1574,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Service Time Per Item'!$G$3:$G$89</c:f>
+              <c:f>'Self-Check Time Per Item'!$G$3:$G$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="87"/>
@@ -1841,11 +1853,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1608016320"/>
-        <c:axId val="-1608024480"/>
+        <c:axId val="-1725571840"/>
+        <c:axId val="-1725582176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1608016320"/>
+        <c:axId val="-1725571840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1887,7 +1899,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1608024480"/>
+        <c:crossAx val="-1725582176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1895,7 +1907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1608024480"/>
+        <c:axId val="-1725582176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1946,7 +1958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1608016320"/>
+        <c:crossAx val="-1725571840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2136,10 +2148,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
@@ -2161,11 +2173,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1373310320"/>
-        <c:axId val="-1373317392"/>
+        <c:axId val="-1725570208"/>
+        <c:axId val="-1725580000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373310320"/>
+        <c:axId val="-1725570208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2219,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373317392"/>
+        <c:crossAx val="-1725580000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2215,7 +2227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373317392"/>
+        <c:axId val="-1725580000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2266,7 +2278,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373310320"/>
+        <c:crossAx val="-1725570208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2450,7 +2462,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -2544,11 +2556,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1373305968"/>
-        <c:axId val="-1373319024"/>
+        <c:axId val="-1725581632"/>
+        <c:axId val="-1725570752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373305968"/>
+        <c:axId val="-1725581632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2590,7 +2602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373319024"/>
+        <c:crossAx val="-1725570752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2598,7 +2610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373319024"/>
+        <c:axId val="-1725570752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2649,7 +2661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373305968"/>
+        <c:crossAx val="-1725581632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2833,16 +2845,16 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
@@ -2927,11 +2939,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1373317936"/>
-        <c:axId val="-1373316848"/>
+        <c:axId val="-1725571296"/>
+        <c:axId val="-1725579456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373317936"/>
+        <c:axId val="-1725571296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2973,7 +2985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373316848"/>
+        <c:crossAx val="-1725579456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2981,7 +2993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373316848"/>
+        <c:axId val="-1725579456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3032,7 +3044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373317936"/>
+        <c:crossAx val="-1725571296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3601,11 +3613,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1373315760"/>
-        <c:axId val="-1373314672"/>
+        <c:axId val="-1725581088"/>
+        <c:axId val="-1725578368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373315760"/>
+        <c:axId val="-1725581088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3702,7 +3714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373314672"/>
+        <c:crossAx val="-1725578368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3711,7 +3723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373314672"/>
+        <c:axId val="-1725578368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3817,7 +3829,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373315760"/>
+        <c:crossAx val="-1725581088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3958,7 +3970,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Service Time Per Item'!$G$3:$G$89</c:f>
+              <c:f>'Self-Check Time Per Item'!$G$3:$G$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="87"/>
@@ -4237,11 +4249,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1373313040"/>
-        <c:axId val="-1373315216"/>
+        <c:axId val="-98180768"/>
+        <c:axId val="-98174240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373313040"/>
+        <c:axId val="-98180768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4283,7 +4295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373315216"/>
+        <c:crossAx val="-98174240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4291,7 +4303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373315216"/>
+        <c:axId val="-98174240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4342,7 +4354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373313040"/>
+        <c:crossAx val="-98180768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4532,10 +4544,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
@@ -4557,11 +4569,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1373321200"/>
-        <c:axId val="-1373308144"/>
+        <c:axId val="-98176416"/>
+        <c:axId val="-98166624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373321200"/>
+        <c:axId val="-98176416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4603,7 +4615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373308144"/>
+        <c:crossAx val="-98166624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4611,7 +4623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373308144"/>
+        <c:axId val="-98166624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4662,7 +4674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373321200"/>
+        <c:crossAx val="-98176416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4846,7 +4858,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -4940,11 +4952,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1373320656"/>
-        <c:axId val="-1373314128"/>
+        <c:axId val="-98172608"/>
+        <c:axId val="-98179136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373320656"/>
+        <c:axId val="-98172608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4986,7 +4998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373314128"/>
+        <c:crossAx val="-98179136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4994,7 +5006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373314128"/>
+        <c:axId val="-98179136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5045,7 +5057,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373320656"/>
+        <c:crossAx val="-98172608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11119,8 +11131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J249"/>
   <sheetViews>
-    <sheetView topLeftCell="A232" workbookViewId="0">
-      <selection sqref="A1:B239"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -12887,10 +12899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="H2" sqref="H2:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -12899,11 +12911,11 @@
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
+    <row r="1" spans="2:11">
       <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
@@ -12917,7 +12929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:11">
       <c r="B2">
         <v>722</v>
       </c>
@@ -12931,8 +12943,9 @@
         <f>D2/60</f>
         <v>16.238333333333333</v>
       </c>
-    </row>
-    <row r="3" spans="2:5">
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="2:11">
       <c r="B3">
         <v>252</v>
       </c>
@@ -12943,11 +12956,13 @@
         <v>470.3</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E27" si="0">D3/60</f>
+        <f t="shared" ref="E3:E26" si="0">D3/60</f>
         <v>7.8383333333333338</v>
       </c>
-    </row>
-    <row r="4" spans="2:5">
+      <c r="H3" s="24"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="2:11">
       <c r="B4">
         <v>964</v>
       </c>
@@ -12961,8 +12976,10 @@
         <f t="shared" si="0"/>
         <v>12.353333333333333</v>
       </c>
-    </row>
-    <row r="5" spans="2:5">
+      <c r="H4" s="24"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="2:11">
       <c r="B5">
         <v>95</v>
       </c>
@@ -12976,8 +12993,10 @@
         <f t="shared" si="0"/>
         <v>17.436666666666667</v>
       </c>
-    </row>
-    <row r="6" spans="2:5">
+      <c r="H5" s="24"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6">
         <v>1547</v>
       </c>
@@ -12991,8 +13010,10 @@
         <f t="shared" si="0"/>
         <v>18.673333333333336</v>
       </c>
-    </row>
-    <row r="7" spans="2:5">
+      <c r="H6" s="24"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7">
         <v>92</v>
       </c>
@@ -13006,8 +13027,10 @@
         <f t="shared" si="0"/>
         <v>15.871666666666666</v>
       </c>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="H7" s="24"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="2:11">
       <c r="B8">
         <v>218</v>
       </c>
@@ -13021,8 +13044,10 @@
         <f t="shared" si="0"/>
         <v>21.831666666666667</v>
       </c>
-    </row>
-    <row r="9" spans="2:5">
+      <c r="H8" s="24"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="2:11">
       <c r="B9">
         <v>1006</v>
       </c>
@@ -13036,8 +13061,9 @@
         <f t="shared" si="0"/>
         <v>10.083333333333334</v>
       </c>
-    </row>
-    <row r="10" spans="2:5">
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="2:11">
       <c r="B10">
         <v>168</v>
       </c>
@@ -13051,8 +13077,9 @@
         <f t="shared" si="0"/>
         <v>17.954999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="2:11">
       <c r="B11">
         <v>993</v>
       </c>
@@ -13066,8 +13093,9 @@
         <f t="shared" si="0"/>
         <v>17.936666666666667</v>
       </c>
-    </row>
-    <row r="12" spans="2:5">
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="2:11">
       <c r="B12">
         <v>271</v>
       </c>
@@ -13081,8 +13109,9 @@
         <f t="shared" si="0"/>
         <v>16.27</v>
       </c>
-    </row>
-    <row r="13" spans="2:5">
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="2:11">
       <c r="B13">
         <v>1159</v>
       </c>
@@ -13096,8 +13125,9 @@
         <f t="shared" si="0"/>
         <v>16.215</v>
       </c>
-    </row>
-    <row r="14" spans="2:5">
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="2:11">
       <c r="B14">
         <v>210</v>
       </c>
@@ -13111,8 +13141,9 @@
         <f t="shared" si="0"/>
         <v>22.548333333333336</v>
       </c>
-    </row>
-    <row r="15" spans="2:5">
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="2:11">
       <c r="B15">
         <v>1060</v>
       </c>
@@ -13126,8 +13157,9 @@
         <f t="shared" si="0"/>
         <v>15.1</v>
       </c>
-    </row>
-    <row r="16" spans="2:5">
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="2:11">
       <c r="B16">
         <v>259</v>
       </c>
@@ -13141,8 +13173,9 @@
         <f t="shared" si="0"/>
         <v>15.591666666666667</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="B17">
         <v>1411</v>
       </c>
@@ -13156,8 +13189,9 @@
         <f t="shared" si="0"/>
         <v>15.263333333333332</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="B18">
         <v>374</v>
       </c>
@@ -13171,8 +13205,9 @@
         <f t="shared" si="0"/>
         <v>14.305</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="H18" s="24"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="B19">
         <v>65</v>
       </c>
@@ -13186,8 +13221,9 @@
         <f t="shared" si="0"/>
         <v>18.943333333333332</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="B20">
         <v>113</v>
       </c>
@@ -13201,8 +13237,9 @@
         <f t="shared" si="0"/>
         <v>33.481666666666669</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="H20" s="24"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="B21">
         <v>1103</v>
       </c>
@@ -13216,8 +13253,9 @@
         <f t="shared" si="0"/>
         <v>19.951666666666664</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="H21" s="24"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="B22">
         <v>399</v>
       </c>
@@ -13231,8 +13269,9 @@
         <f t="shared" si="0"/>
         <v>12.073333333333332</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="B23">
         <v>569</v>
       </c>
@@ -13246,8 +13285,9 @@
         <f t="shared" si="0"/>
         <v>21.734999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="H23" s="24"/>
+    </row>
+    <row r="24" spans="1:9">
       <c r="B24">
         <v>34</v>
       </c>
@@ -13261,8 +13301,9 @@
         <f t="shared" si="0"/>
         <v>18.623333333333335</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="H24" s="24"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="B25">
         <v>34</v>
       </c>
@@ -13276,8 +13317,9 @@
         <f t="shared" si="0"/>
         <v>10.19</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="H25" s="24"/>
+    </row>
+    <row r="26" spans="1:9">
       <c r="B26">
         <v>31</v>
       </c>
@@ -13291,47 +13333,41 @@
         <f t="shared" si="0"/>
         <v>10.241666666666667</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27">
-        <v>90</v>
-      </c>
-      <c r="C27">
-        <v>40.1</v>
-      </c>
-      <c r="D27">
-        <v>576.79999999999995</v>
-      </c>
-      <c r="E27" s="7">
-        <f t="shared" si="0"/>
-        <v>9.6133333333333333</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="8" t="s">
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="4">
-        <f>SUM(B2:B27)</f>
-        <v>13239</v>
-      </c>
-      <c r="C28" s="4">
-        <f>AVERAGE(C2:C27)</f>
-        <v>41.284615384615378</v>
-      </c>
-      <c r="D28" s="4">
-        <f>AVERAGE(D2:D27)</f>
-        <v>983.91923076923081</v>
-      </c>
-      <c r="E28" s="9">
-        <f>AVERAGE(E2:E27)</f>
-        <v>16.398653846153849</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="E29" s="5"/>
+      <c r="B27" s="4">
+        <f>SUM(B2:B26)</f>
+        <v>13149</v>
+      </c>
+      <c r="C27" s="4">
+        <f>AVERAGE(C2:C26)</f>
+        <v>41.332000000000001</v>
+      </c>
+      <c r="D27" s="4">
+        <f>AVERAGE(D2:D26)</f>
+        <v>1000.2040000000001</v>
+      </c>
+      <c r="E27" s="9">
+        <f>AVERAGE(E2:E26)</f>
+        <v>16.670066666666671</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="E28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="24"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="H29" s="5"/>
     </row>
   </sheetData>
+  <sortState ref="H2:H27">
+    <sortCondition ref="H2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -13341,8 +13377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I239"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -15493,7 +15529,7 @@
   <dimension ref="A1:S89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -15501,6 +15537,7 @@
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -15515,15 +15552,22 @@
         <f>AVERAGE(A2:A45)</f>
         <v>28.818181818181817</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2">
         <f>ROUND(EVERYTHING!G11,0)</f>
         <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <f>_xlfn.STDEV.S(A2:A45)</f>
+        <v>20.430566165102682</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>29</v>
@@ -16543,7 +16587,8 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16551,8 +16596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -16576,13 +16621,13 @@
       </c>
       <c r="D1" s="14">
         <f>AVERAGE(A2:A45)</f>
-        <v>6.1136363636363633</v>
+        <v>6.0909090909090908</v>
       </c>
       <c r="E1" s="10"/>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
@@ -16598,19 +16643,26 @@
       <c r="R1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="T1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="26"/>
-      <c r="Y1" s="24" t="s">
+      <c r="U1" s="28"/>
+      <c r="Y1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="24"/>
+      <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2">
         <v>1</v>
       </c>
+      <c r="C2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <f>_xlfn.STDEV.S(A2:A45)</f>
+        <v>4.6195649740730866</v>
+      </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
@@ -16710,6 +16762,10 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
+      <c r="D5">
+        <f>_xlfn.STDEV.S(A2:A37)</f>
+        <v>2.5254262566501078</v>
+      </c>
       <c r="F5">
         <v>3</v>
       </c>
@@ -17104,14 +17160,14 @@
       </c>
       <c r="U16">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="5">
         <v>14</v>
       </c>
       <c r="Z16" s="5">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:33">
@@ -17157,7 +17213,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18">
         <f>'Cashier Data'!D18/'Cashier Data'!C18</f>
@@ -17179,7 +17235,7 @@
       </c>
       <c r="Z18" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:33">
@@ -17191,7 +17247,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q19">
         <f>'Cashier Data'!D19/'Cashier Data'!C19</f>
@@ -17213,7 +17269,7 @@
       </c>
       <c r="Z19" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:33">
@@ -17465,13 +17521,13 @@
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="Q27">
-        <f>'Cashier Data'!D27/'Cashier Data'!C27</f>
-        <v>14.384039900249375</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="0"/>
-        <v>14</v>
+      <c r="Q27" t="e">
+        <f>'Cashier Data'!#REF!/'Cashier Data'!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R27" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="T27">
         <v>25</v>
@@ -17526,9 +17582,9 @@
       <c r="Q29" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="R29" s="18">
+      <c r="R29" s="18" t="e">
         <f>AVERAGE(R2:R27)</f>
-        <v>24</v>
+        <v>#REF!</v>
       </c>
       <c r="T29">
         <v>27</v>
@@ -17555,6 +17611,13 @@
       <c r="G30">
         <v>0</v>
       </c>
+      <c r="Q30" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="R30" s="18" t="e">
+        <f>_xlfn.STDEV.S(R2:R27)</f>
+        <v>#REF!</v>
+      </c>
       <c r="T30">
         <v>28</v>
       </c>
@@ -17851,7 +17914,7 @@
     </row>
     <row r="43" spans="1:26">
       <c r="A43" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:26">
@@ -17884,7 +17947,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -17899,9 +17962,9 @@
         <v>31</v>
       </c>
       <c r="B1" s="18">
-        <v>20.344537819999999</v>
-      </c>
-      <c r="C1" s="27" t="s">
+        <v>22.483193277310924</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="15" t="s">
@@ -17918,7 +17981,7 @@
       <c r="B2" s="18">
         <v>28.818180000000002</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="29"/>
       <c r="E2" s="15" t="s">
         <v>34</v>
       </c>
@@ -17933,7 +17996,7 @@
       <c r="B3" s="18">
         <v>0.27331100000000003</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="15" t="s">

</xml_diff>

<commit_message>
Simulation is finished and works as intended (to my knowledge)
</commit_message>
<xml_diff>
--- a/Giant Eagle Data Stuff.xlsx
+++ b/Giant Eagle Data Stuff.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EVERYTHING" sheetId="1" r:id="rId1"/>
@@ -833,11 +833,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1725583264"/>
-        <c:axId val="-1725569664"/>
+        <c:axId val="146200656"/>
+        <c:axId val="463266832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1725583264"/>
+        <c:axId val="146200656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +934,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725569664"/>
+        <c:crossAx val="463266832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -943,7 +943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1725569664"/>
+        <c:axId val="463266832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1049,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725583264"/>
+        <c:crossAx val="146200656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1328,11 +1328,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1962262608"/>
-        <c:axId val="-1962260976"/>
+        <c:axId val="467777280"/>
+        <c:axId val="467775104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1962262608"/>
+        <c:axId val="467777280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1374,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962260976"/>
+        <c:crossAx val="467775104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1382,7 +1382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962260976"/>
+        <c:axId val="467775104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1433,7 +1433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962262608"/>
+        <c:crossAx val="467777280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1853,11 +1853,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1725571840"/>
-        <c:axId val="-1725582176"/>
+        <c:axId val="463264112"/>
+        <c:axId val="463258672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1725571840"/>
+        <c:axId val="463264112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,7 +1899,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725582176"/>
+        <c:crossAx val="463258672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1907,7 +1907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1725582176"/>
+        <c:axId val="463258672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,7 +1958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725571840"/>
+        <c:crossAx val="463264112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2173,11 +2173,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1725570208"/>
-        <c:axId val="-1725580000"/>
+        <c:axId val="463272816"/>
+        <c:axId val="463270640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1725570208"/>
+        <c:axId val="463272816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2219,7 +2219,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725580000"/>
+        <c:crossAx val="463270640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2227,7 +2227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1725580000"/>
+        <c:axId val="463270640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +2278,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725570208"/>
+        <c:crossAx val="463272816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2556,11 +2556,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1725581632"/>
-        <c:axId val="-1725570752"/>
+        <c:axId val="463273904"/>
+        <c:axId val="463261392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1725581632"/>
+        <c:axId val="463273904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2602,7 +2602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725570752"/>
+        <c:crossAx val="463261392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2610,7 +2610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1725570752"/>
+        <c:axId val="463261392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2661,7 +2661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725581632"/>
+        <c:crossAx val="463273904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2939,11 +2939,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1725571296"/>
-        <c:axId val="-1725579456"/>
+        <c:axId val="463260304"/>
+        <c:axId val="463268464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1725571296"/>
+        <c:axId val="463260304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2985,7 +2985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725579456"/>
+        <c:crossAx val="463268464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2993,7 +2993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1725579456"/>
+        <c:axId val="463268464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,7 +3044,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725571296"/>
+        <c:crossAx val="463260304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3613,11 +3613,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1725581088"/>
-        <c:axId val="-1725578368"/>
+        <c:axId val="463269552"/>
+        <c:axId val="463263024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1725581088"/>
+        <c:axId val="463269552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3714,7 +3714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725578368"/>
+        <c:crossAx val="463263024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3723,7 +3723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1725578368"/>
+        <c:axId val="463263024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3829,7 +3829,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725581088"/>
+        <c:crossAx val="463269552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4249,11 +4249,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-98180768"/>
-        <c:axId val="-98174240"/>
+        <c:axId val="463266288"/>
+        <c:axId val="463263568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-98180768"/>
+        <c:axId val="463266288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4295,7 +4295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-98174240"/>
+        <c:crossAx val="463263568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4303,7 +4303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-98174240"/>
+        <c:axId val="463263568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4354,7 +4354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-98180768"/>
+        <c:crossAx val="463266288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4569,11 +4569,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-98176416"/>
-        <c:axId val="-98166624"/>
+        <c:axId val="463269008"/>
+        <c:axId val="467765856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-98176416"/>
+        <c:axId val="463269008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4615,7 +4615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-98166624"/>
+        <c:crossAx val="467765856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4623,7 +4623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-98166624"/>
+        <c:axId val="467765856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4674,7 +4674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-98176416"/>
+        <c:crossAx val="463269008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4952,11 +4952,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-98172608"/>
-        <c:axId val="-98179136"/>
+        <c:axId val="467763680"/>
+        <c:axId val="467766400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-98172608"/>
+        <c:axId val="467763680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4998,7 +4998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-98179136"/>
+        <c:crossAx val="467766400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5006,7 +5006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-98179136"/>
+        <c:axId val="467766400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5057,7 +5057,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-98172608"/>
+        <c:crossAx val="467763680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12901,8 +12901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:L29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -15528,7 +15528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>